<commit_message>
care table and cards added to tableau
</commit_message>
<xml_diff>
--- a/care.xlsx
+++ b/care.xlsx
@@ -14,12 +14,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>total</t>
   </si>
   <si>
     <t>média/animal</t>
+  </si>
+  <si>
+    <t>tratamentos sarna</t>
+  </si>
+  <si>
+    <t>tratamentos pulga</t>
+  </si>
+  <si>
+    <t>vacinas</t>
+  </si>
+  <si>
+    <t>vermífugos</t>
+  </si>
+  <si>
+    <t>dias de internação</t>
   </si>
 </sst>
 </file>
@@ -377,57 +392,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
         <v>16068</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
         <v>15980</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
         <v>1864</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
         <v>6019</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
         <v>6414</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>6</v>
       </c>
     </row>

</xml_diff>